<commit_message>
Změněny názvy parametrů v error.php
Provizorní CSV tabulky opraveny podle zadání
</commit_message>
<xml_diff>
--- a/sql/import.xlsx
+++ b/sql/import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvori\OneDrive\Documents\nahradni-hodnoceni\sql\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pveris\Documents\Projects\nahradni-hodnoceni\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCFCFF33-EB08-402B-9174-30F9EF5E2B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2854D966-8190-43FB-AD29-C51D757DFDBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11844" yWindow="5292" windowWidth="17280" windowHeight="8964"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>třída</t>
   </si>
@@ -83,28 +83,25 @@
     <t>Holý</t>
   </si>
   <si>
-    <t>Informatika</t>
-  </si>
-  <si>
-    <t>Programování</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Libor Bajer</t>
-  </si>
-  <si>
-    <t>Zdeněk Šilar</t>
-  </si>
-  <si>
-    <t>Ladislav Štěpánek</t>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>PG</t>
+  </si>
+  <si>
+    <t>Bajer</t>
+  </si>
+  <si>
+    <t>Šilar</t>
+  </si>
+  <si>
+    <t>Štěpánek</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -139,7 +136,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -155,7 +152,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -443,27 +440,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,7 +480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -500,10 +497,10 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -520,10 +517,10 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -536,11 +533,11 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
-        <v>17</v>
+      <c r="E4">
+        <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>